<commit_message>
Atualizacao de planilha de importacao
</commit_message>
<xml_diff>
--- a/teste 2.xlsx
+++ b/teste 2.xlsx
@@ -9,24 +9,12 @@
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>classificação</t>
   </si>
@@ -46,31 +34,46 @@
     <t>status</t>
   </si>
   <si>
-    <t>bladasodaçld</t>
-  </si>
-  <si>
-    <t>\djlsçk</t>
-  </si>
-  <si>
-    <t>aslkdjsalkdj</t>
-  </si>
-  <si>
-    <t>kdsljdk</t>
-  </si>
-  <si>
-    <t>saçjsdhlksajd</t>
-  </si>
-  <si>
-    <t>çldskhdkl</t>
-  </si>
-  <si>
-    <t>çlsakjdlks</t>
-  </si>
-  <si>
-    <t>lsakjds</t>
-  </si>
-  <si>
     <t>29/02/2017</t>
+  </si>
+  <si>
+    <t>a0123</t>
+  </si>
+  <si>
+    <t>a0124</t>
+  </si>
+  <si>
+    <t>a0125</t>
+  </si>
+  <si>
+    <t>a0126</t>
+  </si>
+  <si>
+    <t>a0127</t>
+  </si>
+  <si>
+    <t>a0128</t>
+  </si>
+  <si>
+    <t>a0129</t>
+  </si>
+  <si>
+    <t>a0130</t>
+  </si>
+  <si>
+    <t>Banco do Brasil</t>
+  </si>
+  <si>
+    <t>Santander</t>
+  </si>
+  <si>
+    <t>Caixa Economica Federal</t>
+  </si>
+  <si>
+    <t>Pago</t>
+  </si>
+  <si>
+    <t>Não Pago</t>
   </si>
 </sst>
 </file>
@@ -94,7 +97,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -102,19 +105,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -414,113 +461,198 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Plan1"/>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1232</v>
+      </c>
+      <c r="B2" s="2">
+        <v>42786</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1">
+        <v>23.4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>32345</v>
+      </c>
+      <c r="B3" s="2">
+        <v>42770</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1">
+        <v>50</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>12324</v>
+      </c>
+      <c r="B4" s="2">
+        <v>42775</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1">
+        <v>32.54</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>99533</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1000.45</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>1232</v>
       </c>
-      <c r="B2" s="1">
-        <v>42786</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>23.4</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="B6" s="2">
+        <v>42768</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1">
+        <v>15.4</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>32345</v>
       </c>
-      <c r="B3" s="1">
-        <v>42770</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B7" s="2">
+        <v>42771</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3">
-        <v>50</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1">
+        <v>30</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>12324</v>
+      </c>
+      <c r="B8" s="2">
+        <v>42774</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>12324</v>
-      </c>
-      <c r="B4" s="1">
-        <v>42775</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="D8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="1">
+        <v>21.09</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>99533</v>
+      </c>
+      <c r="B9" s="2">
+        <v>42794</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4">
-        <v>32.54</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>99533</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5">
-        <v>1000.45</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="D9" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="E9" s="1">
+        <v>54.344999999999999</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização da importação por parâmetros
</commit_message>
<xml_diff>
--- a/teste 2.xlsx
+++ b/teste 2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>classificação</t>
   </si>
@@ -74,6 +74,12 @@
   </si>
   <si>
     <t>Não Pago</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>subtotal</t>
   </si>
 </sst>
 </file>
@@ -461,7 +467,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Plan1"/>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -556,102 +562,122 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>99533</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1000.45</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="A5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>1232</v>
-      </c>
-      <c r="B6" s="2">
-        <v>42768</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="1">
-        <v>15.4</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>32345</v>
-      </c>
-      <c r="B7" s="2">
-        <v>42771</v>
+        <v>99533</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E7" s="1">
-        <v>30</v>
+        <v>1000.45</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>12324</v>
+        <v>1232</v>
       </c>
       <c r="B8" s="2">
-        <v>42774</v>
+        <v>42768</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E8" s="1">
-        <v>21.09</v>
+        <v>15.4</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
+        <v>32345</v>
+      </c>
+      <c r="B9" s="2">
+        <v>42771</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="1">
+        <v>30</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>12324</v>
+      </c>
+      <c r="B10" s="2">
+        <v>42774</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="1">
+        <v>21.09</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>99533</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B11" s="2">
         <v>42794</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E11" s="1">
         <v>54.344999999999999</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização da planilha de importar_Com_Parametro
</commit_message>
<xml_diff>
--- a/teste 2.xlsx
+++ b/teste 2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>classificação</t>
   </si>
@@ -80,6 +80,24 @@
   </si>
   <si>
     <t>subtotal</t>
+  </si>
+  <si>
+    <t>qqqq1</t>
+  </si>
+  <si>
+    <t>yuyuyu666</t>
+  </si>
+  <si>
+    <t>686868efjf</t>
+  </si>
+  <si>
+    <t>fkrioi5</t>
+  </si>
+  <si>
+    <t>oti5o4oi</t>
+  </si>
+  <si>
+    <t>oi5pir</t>
   </si>
 </sst>
 </file>
@@ -502,8 +520,8 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1232</v>
+      <c r="A2" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="B2" s="2">
         <v>42786</v>
@@ -523,7 +541,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>32345</v>
+        <v>343442</v>
       </c>
       <c r="B3" s="2">
         <v>42770</v>
@@ -542,8 +560,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>12324</v>
+      <c r="A4" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="B4" s="2">
         <v>42775</v>
@@ -582,8 +600,8 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>99533</v>
+      <c r="A7" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
@@ -602,8 +620,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>1232</v>
+      <c r="A8" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="B8" s="2">
         <v>42768</v>
@@ -622,8 +640,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>32345</v>
+      <c r="A9" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="B9" s="2">
         <v>42771</v>
@@ -642,8 +660,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>12324</v>
+      <c r="A10" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="B10" s="2">
         <v>42774</v>
@@ -663,7 +681,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>99533</v>
+        <v>767</v>
       </c>
       <c r="B11" s="2">
         <v>42794</v>

</xml_diff>